<commit_message>
refactor(translation): added manually verified translation
</commit_message>
<xml_diff>
--- a/utils/localisation_script/excel_to_json/as/zlatest.xlsx
+++ b/utils/localisation_script/excel_to_json/as/zlatest.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sreejithv/TW/projects/ekStep/crowdsource-dataplatform/utils/localisation_script/excel_to_json/as/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nireshkumarr/Documents/ekstep/crowdsource-dataplatform/utils/localisation_script/excel_to_json/as/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E232A031-533D-3046-AA18-ED232E7F7A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE65F1BA-5F6B-204C-B197-6EDE2B6882CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{8A6112F6-1D47-BF40-B99F-3DB2AA07C7EB}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20400" xr2:uid="{8A6112F6-1D47-BF40-B99F-3DB2AA07C7EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -222,9 +222,6 @@
     <t>ত্ৰুটি</t>
   </si>
   <si>
-    <t>Start typing here</t>
-  </si>
-  <si>
     <t>ইয়াত টাইপ কৰা আৰম্ভ কৰক</t>
   </si>
   <si>
@@ -264,12 +261,6 @@
     <t>আপোনাৰ মতামতে দেখো ইণ্ডিয়াক প্ৰাসংগিক কৰি ৰখাত সহায় কৰে, আমি আপোনাক মতামত দিবলৈ লোৱা সময়ৰ বাবে প্ৰশংসা কৰো।</t>
   </si>
   <si>
-    <t>Your next goal is to reach &lt;span id=\"next_badge_count\"&gt;&lt;/span&gt; images to earn your &lt;span id=\"next_badge_name_1\"&gt;&lt;/span&gt; Bhasha Samarthak Badge. &lt;a href=\"./badges.html\"&gt;Know more&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>আপোনাৰ পৰৱৰ্তী লক্ষ্য হৈছে &lt;span id=\"next_badge_count\"&gt;&lt;/span&gt; ছবিত উপনীত হৈ আপোনাৰ &lt;span id=\"next_badge_name_1\"&gt;&lt;/span&gt; ভাষা সমৰ্থক বেজ অৰ্জন কৰা। &lt;a href=\"./badges.html\"&gt;অধিক জানক&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Contribute your voice by recording the sentence</t>
   </si>
   <si>
@@ -288,12 +279,6 @@
     <t>ডেচবোৰ্ড</t>
   </si>
   <si>
-    <t>By proceeding ahead you agree to the &lt;a href=\"../terms-and-conditions.html\" target=\"_blank\"&gt; Terms and Conditions&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>আগবাঢ়ি গৈ আপুনি &lt;a href=\"../terms-and-conditions.html\" target=\"_blank\"&gt; চৰ্তাৱলী আৰু নিয়মাৱলীৰ&lt;/a&gt; সৈতে সন্মত হৈছে</t>
-  </si>
-  <si>
     <t>Submitted successfully</t>
   </si>
   <si>
@@ -304,6 +289,21 @@
   </si>
   <si>
     <t>আপোনাৰ মতামতৰ বাবে আপোনাক ধন্যবাদ!</t>
+  </si>
+  <si>
+    <t>Your next goal is to reach &lt;span id="next_badge_count"&gt;&lt;/span&gt; images to earn your &lt;span id="next_badge_name_1"&gt;&lt;/span&gt; Bhasha Samarthak Badge. &lt;a href="./badges.html"&gt;Know more&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>আপোনাৰ পৰৱৰ্তী লক্ষ্য হৈছে &lt;span id="next_badge_count"&gt;&lt;/span&gt; ছবিত উপনীত হৈ আপোনাৰ &lt;span id="next_badge_name_1"&gt;&lt;/span&gt; ভাষা সমৰ্থক বেজ অৰ্জন কৰা। &lt;a href="./badges.html"&gt;অধিক জানক&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>By proceeding ahead you agree to the &lt;a href="../terms-and-conditions.html" target="_blank"&gt; Terms and Conditions&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>আগবাঢ়ি গৈ আপুনি &lt;a href="../terms-and-conditions.html" target="_blank"&gt; চৰ্তাৱলী আৰু নিয়মাৱলীৰ&lt;/a&gt; সৈতে সন্মত হৈছে</t>
+  </si>
+  <si>
+    <t>Start typing here...</t>
   </si>
 </sst>
 </file>
@@ -699,7 +699,7 @@
   <dimension ref="A1:Z1009"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -923,11 +923,11 @@
     <row r="8" spans="1:26">
       <c r="A8" s="1"/>
       <c r="B8" s="3" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -955,11 +955,11 @@
     <row r="9" spans="1:26">
       <c r="A9" s="1"/>
       <c r="B9" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -987,11 +987,11 @@
     <row r="10" spans="1:26">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -1019,11 +1019,11 @@
     <row r="11" spans="1:26">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -1051,11 +1051,11 @@
     <row r="12" spans="1:26">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -1083,11 +1083,11 @@
     <row r="13" spans="1:26">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1115,11 +1115,11 @@
     <row r="14" spans="1:26">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -1979,11 +1979,11 @@
     <row r="41" spans="1:26">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="4" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -2011,11 +2011,11 @@
     <row r="42" spans="1:26">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -2043,11 +2043,11 @@
     <row r="43" spans="1:26">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -2075,11 +2075,11 @@
     <row r="44" spans="1:26">
       <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -2107,11 +2107,11 @@
     <row r="45" spans="1:26">
       <c r="A45" s="1"/>
       <c r="B45" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="4" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -2139,11 +2139,11 @@
     <row r="46" spans="1:26">
       <c r="A46" s="1"/>
       <c r="B46" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="4" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -2171,11 +2171,11 @@
     <row r="47" spans="1:26">
       <c r="A47" s="1"/>
       <c r="B47" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>

</xml_diff>